<commit_message>
P4-Added Refactoring and Design Pattern List. Updated traceability link matrix.
</commit_message>
<xml_diff>
--- a/Traceability_Link_Matrix.xlsx
+++ b/Traceability_Link_Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="34">
   <si>
     <t>SecurityController</t>
   </si>
@@ -23,6 +23,9 @@
     <t>UserController</t>
   </si>
   <si>
+    <t>WorkoutController</t>
+  </si>
+  <si>
     <t>HibernatePersistenceService</t>
   </si>
   <si>
@@ -41,10 +44,37 @@
     <t>Trainer</t>
   </si>
   <si>
-    <t>Customer </t>
-  </si>
-  <si>
-    <t>Session</t>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Enum_Role</t>
+  </si>
+  <si>
+    <t>EquipmentItem</t>
+  </si>
+  <si>
+    <t>Exercise</t>
+  </si>
+  <si>
+    <t>ExerciseSet</t>
+  </si>
+  <si>
+    <t>HealthInsuranceProvider</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>UserInformation</t>
+  </si>
+  <si>
+    <t>WorkoutRoutine</t>
   </si>
   <si>
     <t>UC-1 – Hire Trainer</t>
@@ -56,31 +86,31 @@
     <t>UC-2 -  Register Customer</t>
   </si>
   <si>
-    <t>UC-3</t>
-  </si>
-  <si>
-    <t>UC-4</t>
-  </si>
-  <si>
-    <t>UC-5</t>
-  </si>
-  <si>
-    <t>UC-6</t>
-  </si>
-  <si>
-    <t>UC-7</t>
-  </si>
-  <si>
-    <t>UC-8</t>
-  </si>
-  <si>
-    <t>UC-9</t>
-  </si>
-  <si>
-    <t>UC-10</t>
-  </si>
-  <si>
-    <t>UC-11</t>
+    <t>UC-3 – Inventory Equipment</t>
+  </si>
+  <si>
+    <t>UC-4 – Modify Trainer</t>
+  </si>
+  <si>
+    <t>UC-5 – Modify Customer</t>
+  </si>
+  <si>
+    <t>UC-6 – Modify Equipment Inventory</t>
+  </si>
+  <si>
+    <t>UC-7 – Create Workout Routine</t>
+  </si>
+  <si>
+    <t>UC-8 – Modify Workout Routine</t>
+  </si>
+  <si>
+    <t>UC-9 – Assign Workout Routine</t>
+  </si>
+  <si>
+    <t>UC-10 – Search for Customer</t>
+  </si>
+  <si>
+    <t>UC-11 – Search for Workout Routine</t>
   </si>
   <si>
     <r>
@@ -92,6 +122,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -101,21 +132,13 @@
         <color rgb="FF00000A"/>
         <rFont val="Calibri"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Log in User</t>
     </r>
   </si>
   <si>
-    <t>UC-13</t>
-  </si>
-  <si>
-    <t>UC-14</t>
-  </si>
-  <si>
-    <t>UC-15</t>
-  </si>
-  <si>
-    <t>UC-16</t>
+    <t>UC-13 – Create User Account</t>
   </si>
 </sst>
 </file>
@@ -125,11 +148,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,22 +171,18 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Monospace"/>
-      <family val="0"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF00000A"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,10 +241,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -305,25 +321,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N7" activeCellId="0" sqref="N7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.3265306122449"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="26.1632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="38.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="38.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.3010204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.75"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="20.6989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -351,132 +375,473 @@
       <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+      <c r="O4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="B5" s="0"/>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="O7" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="O8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
+      <c r="O9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="0"/>
+      <c r="K10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="U10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B11" s="0"/>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="K11" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="U12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="T14" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made final modifications to documentation. Domain Model model glossary now in ascending alphabetical order. Package diagram now shows interactions between subpackages. Added final use cases to Tracability link matrix. Added search for trainers and equipment items test cases to the testing document. Refactored Trainer and Customer constructors to follow the builder pattern.
</commit_message>
<xml_diff>
--- a/Traceability_Link_Matrix.xlsx
+++ b/Traceability_Link_Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
   <si>
     <t>SecurityController</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>UC-13 – Create User Account</t>
+  </si>
+  <si>
+    <t>UC-14 – Modify User Account</t>
+  </si>
+  <si>
+    <t>UC-15 – Search for Trainers</t>
+  </si>
+  <si>
+    <t>UC-16 – Search for Equipment Items</t>
   </si>
 </sst>
 </file>
@@ -321,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -480,6 +489,7 @@
       <c r="I3" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="J3" s="0"/>
       <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
@@ -520,6 +530,8 @@
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="0"/>
+      <c r="J4" s="0"/>
+      <c r="K4" s="0"/>
       <c r="O4" s="3" t="s">
         <v>21</v>
       </c>
@@ -551,6 +563,7 @@
       <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="K5" s="0"/>
       <c r="L5" s="3" t="s">
         <v>21</v>
       </c>
@@ -594,6 +607,7 @@
       <c r="I6" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="J6" s="0"/>
       <c r="K6" s="3" t="s">
         <v>21</v>
       </c>
@@ -637,6 +651,8 @@
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
       <c r="O7" s="3" t="s">
         <v>21</v>
       </c>
@@ -659,6 +675,8 @@
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
       <c r="O8" s="3" t="s">
         <v>21</v>
       </c>
@@ -690,6 +708,8 @@
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
       <c r="I9" s="0"/>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
       <c r="O9" s="3" t="s">
         <v>21</v>
       </c>
@@ -723,6 +743,7 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
       <c r="K10" s="3" t="s">
         <v>21</v>
       </c>
@@ -750,6 +771,7 @@
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
       <c r="K11" s="3" t="s">
         <v>21</v>
       </c>
@@ -770,6 +792,8 @@
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
       <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
       <c r="U12" s="3" t="s">
         <v>21</v>
       </c>
@@ -815,7 +839,8 @@
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -841,6 +866,69 @@
       </c>
       <c r="L14" s="3"/>
       <c r="T14" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="O17" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated testing document, development manual, and TLM for the Fitness Class addition.
</commit_message>
<xml_diff>
--- a/Traceability_Link_Matrix.xlsx
+++ b/Traceability_Link_Matrix.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="40">
   <si>
     <t>SecurityController</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>WorkoutRoutine</t>
+  </si>
+  <si>
+    <t>FitnessClass</t>
   </si>
   <si>
     <t>UC-1 – Hire Trainer</t>
@@ -148,6 +151,12 @@
   </si>
   <si>
     <t>UC-16 – Search for Equipment Items</t>
+  </si>
+  <si>
+    <t>UC-17 – Add Fitness Class</t>
+  </si>
+  <si>
+    <t>UC-18 – Modify Fitness Class</t>
   </si>
 </sst>
 </file>
@@ -330,10 +339,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U17"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -417,115 +426,118 @@
       <c r="U1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="V1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
@@ -533,120 +545,120 @@
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
       <c r="O4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0"/>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K5" s="0"/>
       <c r="L5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0"/>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0"/>
       <c r="H7" s="0"/>
@@ -654,23 +666,23 @@
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
       <c r="O7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0"/>
       <c r="C8" s="0"/>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="0"/>
       <c r="H8" s="0"/>
@@ -678,32 +690,32 @@
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
       <c r="O8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0"/>
       <c r="C9" s="0"/>
       <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="0"/>
       <c r="H9" s="0"/>
@@ -711,82 +723,82 @@
       <c r="J9" s="0"/>
       <c r="K9" s="0"/>
       <c r="O9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0"/>
       <c r="C10" s="0"/>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="0"/>
       <c r="J10" s="0"/>
       <c r="K10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="U10" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
       <c r="K11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="0"/>
@@ -795,141 +807,200 @@
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
       <c r="U12" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D14" s="0"/>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L14" s="3"/>
       <c r="T14" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D15" s="0"/>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D16" s="0"/>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3"/>
       <c r="O17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="V18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="V19" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>